<commit_message>
Refactored SciKitSVM.py and introduced synthetic data, will run first test.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tricide\Documents\School\EXTENDED ESSAY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6806FA40-73BC-457F-A364-90F3035A3353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3C6467-3664-4B3B-90DA-BE2D4B3A7103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="690" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Dataset</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>ROC_AUC</t>
   </si>
 </sst>
 </file>
@@ -385,28 +388,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="5" width="21.140625" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" customWidth="1"/>
-    <col min="12" max="12" width="27.28515625" customWidth="1"/>
-    <col min="13" max="13" width="27" customWidth="1"/>
-    <col min="14" max="14" width="46.140625" customWidth="1"/>
+    <col min="6" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" customWidth="1"/>
+    <col min="13" max="13" width="27.28515625" customWidth="1"/>
+    <col min="14" max="14" width="27" customWidth="1"/>
+    <col min="15" max="15" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,30 +429,33 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>